<commit_message>
added genotype column earlier in code, removed old excel export lists
</commit_message>
<xml_diff>
--- a/extractions/extractions_master.xlsx
+++ b/extractions/extractions_master.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J294"/>
+  <dimension ref="A1:K294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,6 +415,11 @@
           <t>Temperature</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>geno</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -459,6 +464,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -503,6 +513,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -547,6 +562,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -591,6 +611,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -635,6 +660,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -679,6 +709,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -723,6 +758,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -767,6 +807,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -811,6 +856,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -855,6 +905,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -899,6 +954,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -943,6 +1003,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -987,6 +1052,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1031,6 +1101,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1075,6 +1150,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1119,6 +1199,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1163,6 +1248,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1207,6 +1297,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1251,6 +1346,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1295,6 +1395,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1339,6 +1444,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1383,6 +1493,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1427,6 +1542,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1471,6 +1591,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1515,6 +1640,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1559,6 +1689,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1603,6 +1738,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1647,6 +1787,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1691,6 +1836,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1735,6 +1885,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1779,6 +1934,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1823,6 +1983,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1867,6 +2032,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1911,6 +2081,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1955,6 +2130,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1999,6 +2179,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2043,6 +2228,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2087,6 +2277,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2131,6 +2326,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2175,6 +2375,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2219,6 +2424,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2263,6 +2473,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2307,6 +2522,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2351,6 +2571,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2395,6 +2620,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2439,6 +2669,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2483,6 +2718,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2527,6 +2767,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2571,6 +2816,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2615,6 +2865,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2659,6 +2914,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2703,6 +2963,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2747,6 +3012,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2791,6 +3061,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2835,6 +3110,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2879,6 +3159,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2923,6 +3208,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2967,6 +3257,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3011,6 +3306,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3055,6 +3355,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3099,6 +3404,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3143,6 +3453,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3187,6 +3502,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3231,6 +3551,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3275,6 +3600,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3319,6 +3649,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3363,6 +3698,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3407,6 +3747,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3451,6 +3796,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3495,6 +3845,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3539,6 +3894,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3583,6 +3943,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3627,6 +3992,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3671,6 +4041,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3715,6 +4090,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3759,6 +4139,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3803,6 +4188,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3847,6 +4237,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3891,6 +4286,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3935,6 +4335,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3979,6 +4384,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4023,6 +4433,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4067,6 +4482,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4111,6 +4531,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4155,6 +4580,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4199,6 +4629,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4243,6 +4678,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4287,6 +4727,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4331,6 +4776,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4375,6 +4825,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4419,6 +4874,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4463,6 +4923,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4507,6 +4972,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4551,6 +5021,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4595,6 +5070,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4639,6 +5119,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4683,6 +5168,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4727,6 +5217,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4771,6 +5266,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4815,6 +5315,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4859,6 +5364,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4903,6 +5413,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4947,6 +5462,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4991,6 +5511,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -5035,6 +5560,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -5079,6 +5609,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5123,6 +5658,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5167,6 +5707,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -5211,6 +5756,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5255,6 +5805,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -5299,6 +5854,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5343,6 +5903,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5387,6 +5952,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5431,6 +6001,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5475,6 +6050,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -5519,6 +6099,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5563,6 +6148,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5607,6 +6197,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5651,6 +6246,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5695,6 +6295,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5739,6 +6344,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5783,6 +6393,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5827,6 +6442,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5871,6 +6491,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5915,6 +6540,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5959,6 +6589,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -6003,6 +6638,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -6047,6 +6687,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -6091,6 +6736,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -6135,6 +6785,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -6179,6 +6834,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -6223,6 +6883,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -6267,6 +6932,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -6311,6 +6981,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -6355,6 +7030,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -6399,6 +7079,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -6443,6 +7128,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -6487,6 +7177,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -6531,6 +7226,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -6575,6 +7275,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -6619,6 +7324,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -6663,6 +7373,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -6707,6 +7422,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -6751,6 +7471,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -6795,6 +7520,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6839,6 +7569,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -6883,6 +7618,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -6927,6 +7667,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6971,6 +7716,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -7015,6 +7765,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -7059,6 +7814,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -7103,6 +7863,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -7147,6 +7912,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -7191,6 +7961,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -7235,6 +8010,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -7279,6 +8059,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -7323,6 +8108,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -7367,6 +8157,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -7411,6 +8206,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -7455,6 +8255,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -7499,6 +8304,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -7543,6 +8353,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -7587,6 +8402,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -7631,6 +8451,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -7675,6 +8500,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -7719,6 +8549,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -7763,6 +8598,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -7807,6 +8647,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -7851,6 +8696,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -7895,6 +8745,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -7939,6 +8794,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -7983,6 +8843,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -8027,6 +8892,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -8071,6 +8941,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -8115,6 +8990,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -8159,6 +9039,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -8203,6 +9088,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -8247,6 +9137,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -8291,6 +9186,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -8335,6 +9235,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -8379,6 +9284,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -8423,6 +9333,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -8467,6 +9382,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -8511,6 +9431,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -8555,6 +9480,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -8599,6 +9529,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -8643,6 +9578,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -8687,6 +9627,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -8731,6 +9676,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -8775,6 +9725,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -8819,6 +9774,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -8863,6 +9823,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -8907,6 +9872,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -8951,6 +9921,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -8995,6 +9970,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -9039,6 +10019,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -9083,6 +10068,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -9127,6 +10117,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -9171,6 +10166,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -9215,6 +10215,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -9259,6 +10264,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -9303,6 +10313,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -9347,6 +10362,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -9391,6 +10411,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -9435,6 +10460,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -9479,6 +10509,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -9523,6 +10558,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -9567,6 +10607,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -9611,6 +10656,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -9655,6 +10705,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K211" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -9699,6 +10754,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -9743,6 +10803,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -9787,6 +10852,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -9831,6 +10901,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -9875,6 +10950,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -9919,6 +10999,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -9963,6 +11048,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -10007,6 +11097,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K219" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -10051,6 +11146,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K220" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -10095,6 +11195,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -10139,6 +11244,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K222" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -10183,6 +11293,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K223" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -10227,6 +11342,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K224" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -10271,6 +11391,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K225" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -10315,6 +11440,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K226" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -10359,6 +11489,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K227" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -10403,6 +11538,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K228" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -10447,6 +11587,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K229" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -10491,6 +11636,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K230" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -10535,6 +11685,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K231" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -10579,6 +11734,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K232" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -10623,6 +11783,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K233" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -10667,6 +11832,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K234" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -10711,6 +11881,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K235" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -10755,6 +11930,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K236" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -10799,6 +11979,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K237" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -10843,6 +12028,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K238" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -10887,6 +12077,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K239" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -10931,6 +12126,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K240" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -10975,6 +12175,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K241" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -11019,6 +12224,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K242" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -11063,6 +12273,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K243" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -11107,6 +12322,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K244" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -11151,6 +12371,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K245" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -11195,6 +12420,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K246" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -11239,6 +12469,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K247" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -11283,6 +12518,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K248" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -11327,6 +12567,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K249" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -11371,6 +12616,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K250" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -11415,6 +12665,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K251" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -11459,6 +12714,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K252" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -11503,6 +12763,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K253" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -11547,6 +12812,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K254" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -11591,6 +12861,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K255" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -11635,6 +12910,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K256" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -11679,6 +12959,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K257" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -11723,6 +13008,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K258" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -11767,6 +13057,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K259" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -11811,6 +13106,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K260" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -11855,6 +13155,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K261" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -11899,6 +13204,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K262" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -11943,6 +13253,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K263" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -11987,6 +13302,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K264" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -12031,6 +13351,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K265" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -12075,6 +13400,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K266" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -12119,6 +13449,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K267" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -12163,6 +13498,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K268" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -12207,6 +13547,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K269" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -12251,6 +13596,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K270" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -12295,6 +13645,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K271" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -12339,6 +13694,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K272" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -12383,6 +13743,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K273" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -12427,6 +13792,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K274" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -12471,6 +13841,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K275" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -12515,6 +13890,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K276" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -12559,6 +13939,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K277" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -12603,6 +13988,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K278" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -12647,6 +14037,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K279" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -12691,6 +14086,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K280" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -12735,6 +14135,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K281" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -12779,6 +14184,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K282" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -12823,6 +14233,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K283" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -12867,6 +14282,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K284" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -12911,6 +14331,11 @@
           <t>High</t>
         </is>
       </c>
+      <c r="K285" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -12955,6 +14380,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K286" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -12999,6 +14429,11 @@
           <t>Control</t>
         </is>
       </c>
+      <c r="K287" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -13043,6 +14478,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K288" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -13087,6 +14527,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K289" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -13131,6 +14576,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K290" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -13175,6 +14625,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K291" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -13219,6 +14674,11 @@
           <t>Low</t>
         </is>
       </c>
+      <c r="K292" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -13263,6 +14723,11 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="K293" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -13305,6 +14770,11 @@
       <c r="J294" t="inlineStr">
         <is>
           <t>Medium</t>
+        </is>
+      </c>
+      <c r="K294" t="inlineStr">
+        <is>
+          <t>01</t>
         </is>
       </c>
     </row>

</xml_diff>